<commit_message>
Log addition to check work flow
</commit_message>
<xml_diff>
--- a/Registration files/Test_drive_list.xlsx
+++ b/Registration files/Test_drive_list.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,7 +481,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Yo yo</t>
+          <t>Gul Gulov</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -489,27 +489,27 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Toyota Camry 3</t>
+          <t>Toyota Camry 9</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>15/082025</t>
+          <t>17/082025</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-08-09 11:55:40</t>
+          <t>2025-08-12 11:28:05</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>11:30</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Nothing</t>
         </is>
       </c>
     </row>
@@ -519,15 +519,15 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Yo yo</t>
+          <t>Saidov Khushdil</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>992907510905</v>
+        <v>79177131361</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Toyota Camry 2</t>
+          <t>Toyota Camry 8</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -537,207 +537,17 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-08-09 11:58:47</t>
+          <t>2025-08-12 11:31:01</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>11:30</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>789</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>8138074349</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Toshpulot Toshpulod</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>992556550088</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Toyota Camry 1</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>14/082025</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>2025-08-09 16:20:46</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>11:30</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>8138074349</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Yo yo</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>992907510905</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Toyota Camry 8</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>13/082025</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>2025-08-11 09:29:56</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>15:00</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>8138074349</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Yo yo</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>992907510905</v>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Toyota Camry 5</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>13/082025</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>2025-08-11 10:14:06</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>11:30</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>8138074349</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Yo yo</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>992907510905</v>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Toyota Camry 5</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>15/082025</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>2025-08-11 14:56:58</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>11:30</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>8138074349</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Yo yo</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>992907510905</v>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Toyota Camry 3</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>13/082025</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>2025-08-11 15:00:59</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>11:30</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>-</t>
+          <t>Буду чуть попозже</t>
         </is>
       </c>
     </row>

</xml_diff>